<commit_message>
Complete D4 graph and report
</commit_message>
<xml_diff>
--- a/sprint-backlog/sprint-4/report-sheet.xlsx
+++ b/sprint-backlog/sprint-4/report-sheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184B7209-18CC-4114-8E80-4BC036C770FF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0323FB3-97CB-4B09-AE24-3D25D8029F45}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>Dependency</t>
   </si>
@@ -30,73 +30,85 @@
     <t>Story Points</t>
   </si>
   <si>
-    <t>T3,T4,T6</t>
-  </si>
-  <si>
     <t>J:1</t>
   </si>
   <si>
     <t>K:1</t>
   </si>
   <si>
-    <t>C:1</t>
-  </si>
-  <si>
-    <t>Z:3</t>
-  </si>
-  <si>
     <t>Z:2</t>
   </si>
   <si>
     <t>A:1</t>
   </si>
   <si>
-    <t>A:3</t>
-  </si>
-  <si>
     <t>User Story</t>
   </si>
   <si>
-    <t>K:3</t>
-  </si>
-  <si>
     <t>plan</t>
   </si>
   <si>
     <t>day</t>
   </si>
   <si>
-    <t>Tasks</t>
-  </si>
-  <si>
-    <t>J:4</t>
-  </si>
-  <si>
-    <t>C:5</t>
-  </si>
-  <si>
-    <t>C:2</t>
-  </si>
-  <si>
-    <t>1: 10-23-2018</t>
-  </si>
-  <si>
-    <t>5: 10-27-2018</t>
-  </si>
-  <si>
     <t>J:2</t>
   </si>
   <si>
     <t>J:5</t>
   </si>
   <si>
-    <t>A:5</t>
-  </si>
-  <si>
     <t>C:3</t>
   </si>
   <si>
     <t>actual</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>1: November 7</t>
+  </si>
+  <si>
+    <t>5: November 11</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Z:1</t>
+  </si>
+  <si>
+    <t>J:3</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>K:2</t>
+  </si>
+  <si>
+    <t>A:2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>C:4</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>K:4</t>
+  </si>
+  <si>
+    <t>T24 T25</t>
   </si>
 </sst>
 </file>
@@ -132,9 +144,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,7 +199,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Sprint 2:</a:t>
+              <a:t>Sprint 4:</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
@@ -272,22 +283,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -332,22 +343,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1101,16 +1112,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1653,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1666,10 +1677,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1678,137 +1689,181 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F1">
         <v>2</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1">
         <v>3</v>
       </c>
       <c r="H1">
         <v>4</v>
       </c>
       <c r="I1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>28</v>
+      </c>
+      <c r="D9">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I9" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>29</v>
+      </c>
+      <c r="D10">
         <v>8</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1818,20 +1873,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EF6B04-6D91-4CB2-B795-853A8560DA04}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1840,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F1">
         <v>2</v>
@@ -1852,122 +1907,151 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>27</v>
+      </c>
+      <c r="D8">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>29</v>
+      </c>
+      <c r="D10">
         <v>8</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1979,13 +2063,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D36948-1878-4E62-8F83-9D21899FB0AC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -2008,48 +2094,48 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F2">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F3">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>